<commit_message>
add content to classification paper
</commit_message>
<xml_diff>
--- a/data/raw-data/check_articles.xlsx
+++ b/data/raw-data/check_articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunduniversityo365-my.sharepoint.com/personal/ph8148kr_lu_se/Documents/research/swinno-shades-green/data/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="184" documentId="8_{E07395E0-558C-498F-B5C6-3CDAD76A1923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DC16D69-ABD4-4FCA-8FE5-CB453D5A7616}"/>
+  <xr:revisionPtr revIDLastSave="246" documentId="8_{E07395E0-558C-498F-B5C6-3CDAD76A1923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{846EC08C-2904-47BA-B0AD-FD798EEFAC62}"/>
   <bookViews>
     <workbookView xWindow="-20895" yWindow="0" windowWidth="20895" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="475">
   <si>
     <t>sinno_id</t>
   </si>
@@ -1421,6 +1421,30 @@
   </si>
   <si>
     <t>203,204</t>
+  </si>
+  <si>
+    <t>213,501</t>
+  </si>
+  <si>
+    <t>701,207,201</t>
+  </si>
+  <si>
+    <t>anti bv3</t>
+  </si>
+  <si>
+    <t>not forest</t>
+  </si>
+  <si>
+    <t>non pesticide solution to fighting weevil, but sustainability effects of root removal unsure</t>
+  </si>
+  <si>
+    <t>root cleaner, sustainability unsure</t>
+  </si>
+  <si>
+    <t>good bv 2 example</t>
+  </si>
+  <si>
+    <t>162</t>
   </si>
 </sst>
 </file>
@@ -2310,8 +2334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="G101" sqref="G101"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="H115" sqref="H101:I115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4391,7 +4415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>7726001</v>
       </c>
@@ -4411,7 +4435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>7740001</v>
       </c>
@@ -4437,7 +4461,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="360" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="360" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>7777001</v>
       </c>
@@ -4457,7 +4481,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>7782001</v>
       </c>
@@ -4480,7 +4504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>7796001</v>
       </c>
@@ -4490,8 +4514,20 @@
       <c r="D101" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="E101" s="1">
+        <v>2</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="G101" s="1">
+        <v>1</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>7809001</v>
       </c>
@@ -4501,24 +4537,54 @@
       <c r="D102" s="1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="E102" s="1">
+        <v>9</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="G102" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>7827001</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="E103" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="G103" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>7852001</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+      <c r="E104" s="1">
+        <v>9</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="G104" s="1">
+        <v>1</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>7859001</v>
       </c>
@@ -4528,8 +4594,20 @@
       <c r="D105" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="E105" s="1">
+        <v>9</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="G105" s="1">
+        <v>1</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>7892001</v>
       </c>
@@ -4539,8 +4617,17 @@
       <c r="C106" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="E106" s="1">
+        <v>9</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="G106" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>7897001</v>
       </c>
@@ -4550,8 +4637,20 @@
       <c r="D107" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="E107" s="1">
+        <v>2</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="G107" s="1">
+        <v>1</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>7919001</v>
       </c>
@@ -4564,16 +4663,40 @@
       <c r="D108" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="E108" s="1">
+        <v>2</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="G108" s="1">
+        <v>1</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>7939001</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="E109" s="1">
+        <v>2</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="G109" s="1">
+        <v>1</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>7944001</v>
       </c>
@@ -4583,8 +4706,20 @@
       <c r="C110" s="1" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="E110" s="1">
+        <v>2</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="G110" s="1">
+        <v>1</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>8015001</v>
       </c>
@@ -4594,16 +4729,34 @@
       <c r="C111" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="E111" s="1">
+        <v>9</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="G111" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>8020001</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E112" s="1">
+        <v>2</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="G112" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>8085001</v>
       </c>
@@ -4613,24 +4766,51 @@
       <c r="D113" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="E113" s="1">
+        <v>9</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="G113" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>8122001</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="E114" s="1">
+        <v>2</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="G114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>8129001</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E115" s="1">
+        <v>9</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="G115" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>8149001</v>
       </c>
@@ -4638,7 +4818,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>8167001</v>
       </c>
@@ -4649,7 +4829,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>8193001</v>
       </c>
@@ -4660,7 +4840,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>8193001</v>
       </c>
@@ -4671,7 +4851,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>8238001</v>
       </c>
@@ -4682,7 +4862,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="285" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="285" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>8379001</v>
       </c>
@@ -4693,7 +4873,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>8422001</v>
       </c>
@@ -4701,7 +4881,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>8741001</v>
       </c>
@@ -4712,7 +4892,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>8758001</v>
       </c>
@@ -4723,7 +4903,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>8758001</v>
       </c>
@@ -4734,7 +4914,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>8781001</v>
       </c>
@@ -4745,7 +4925,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>8789001</v>
       </c>
@@ -4756,7 +4936,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>8799001</v>
       </c>

</xml_diff>